<commit_message>
sync code from Developer
221207
</commit_message>
<xml_diff>
--- a/eppEstudio50-main/eppEstudio50-main/nomencladores/excels/tipo_talento.xlsx
+++ b/eppEstudio50-main/eppEstudio50-main/nomencladores/excels/tipo_talento.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enit.Martinez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Enicito\Estudio50\epp\nomencladores\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t> Actores</t>
   </si>
@@ -72,14 +72,157 @@
   </si>
   <si>
     <t>Accesorios</t>
+  </si>
+  <si>
+    <t>Productor</t>
+  </si>
+  <si>
+    <t>Productor ejecutivo</t>
+  </si>
+  <si>
+    <t>Coordinación de producción</t>
+  </si>
+  <si>
+    <t>Director</t>
+  </si>
+  <si>
+    <t>Primer Asistente de Dirección</t>
+  </si>
+  <si>
+    <t>Pizarra</t>
+  </si>
+  <si>
+    <t>Segundo Asistente de Dirección</t>
+  </si>
+  <si>
+    <t>Continuidad</t>
+  </si>
+  <si>
+    <t>Director de Fotografía</t>
+  </si>
+  <si>
+    <t>Primer Asistente de Cámara</t>
+  </si>
+  <si>
+    <t>Segundo Asistente de Cámara</t>
+  </si>
+  <si>
+    <t>Foto Fija</t>
+  </si>
+  <si>
+    <t>Gaffer</t>
+  </si>
+  <si>
+    <t>Director de Arte</t>
+  </si>
+  <si>
+    <t>Coordinador de Arte</t>
+  </si>
+  <si>
+    <t>Decorador</t>
+  </si>
+  <si>
+    <t>Set Decorator</t>
+  </si>
+  <si>
+    <t>Gerente de Locaciones</t>
+  </si>
+  <si>
+    <t>Diseñadora de Vestuario</t>
+  </si>
+  <si>
+    <t>Asistente de vestuario</t>
+  </si>
+  <si>
+    <t>Diseño de Maquillaje y Vestuario</t>
+  </si>
+  <si>
+    <t>Asistente de Maquillaje y Vestuario</t>
+  </si>
+  <si>
+    <t>Armero</t>
+  </si>
+  <si>
+    <t>Taller Pirotécnico</t>
+  </si>
+  <si>
+    <t>Manejador de Animales</t>
+  </si>
+  <si>
+    <t>Director de Sonido</t>
+  </si>
+  <si>
+    <t>Música Original</t>
+  </si>
+  <si>
+    <t>Sonido Directo</t>
+  </si>
+  <si>
+    <t>Editor de Foleys</t>
+  </si>
+  <si>
+    <t>Supervisión Musical</t>
+  </si>
+  <si>
+    <t>Mezclador</t>
+  </si>
+  <si>
+    <t>Asistente de Mezcla</t>
+  </si>
+  <si>
+    <t>Editor de Ambientes y Efectos</t>
+  </si>
+  <si>
+    <t>Coordinador General FX</t>
+  </si>
+  <si>
+    <t>Asistente de Fx</t>
+  </si>
+  <si>
+    <t>Editor</t>
+  </si>
+  <si>
+    <t>Efectos Especiales</t>
+  </si>
+  <si>
+    <t>Diseño Gráfico y Créditos</t>
+  </si>
+  <si>
+    <t>Director de Casting</t>
+  </si>
+  <si>
+    <t>Asistente de Casting</t>
+  </si>
+  <si>
+    <t>Coordinadoras de Casting</t>
+  </si>
+  <si>
+    <t>Coordinadoras de extras</t>
+  </si>
+  <si>
+    <t>Contabilidad</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Transportación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -107,12 +250,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,15 +537,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A15" sqref="A15:A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -576,6 +720,546 @@
         <v>6</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f>A14+1</f>
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f t="shared" ref="A16:A59" si="0">A15+1</f>
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>